<commit_message>
Got fisheries batch 2 ready for test ingest
</commit_message>
<xml_diff>
--- a/datamares/OLR/OLR_datamares_fisheries2.xlsx
+++ b/datamares/OLR/OLR_datamares_fisheries2.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1035" uniqueCount="854">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1008" uniqueCount="845">
   <si>
     <t>text</t>
   </si>
@@ -2053,9 +2053,6 @@
   </si>
   <si>
     <t>2015-04-30</t>
-  </si>
-  <si>
-    <t>f_ug_biological.xlsx</t>
   </si>
   <si>
     <t>Los efectos a corto plazo de las reservas marinas sobre poblaciones de garropas y cabrillas @ http://dx.doi.org/10.13022/M3ZW2S</t>
@@ -2212,9 +2209,6 @@
     <t>Software used: Microsoft Excel; Matlab. Coordinate system: UTM WGS 1984.</t>
   </si>
   <si>
-    <t>f_cp_jacks.xlsx</t>
-  </si>
-  <si>
     <t>Acoustic survey of fish in Cabo Pulmo National Park</t>
   </si>
   <si>
@@ -2261,9 +2255,6 @@
   </si>
   <si>
     <t>Echosounder surveys. This dataset includes the mean lengths of Gulf Corvina per individual echosounder transect across three survey days.</t>
-  </si>
-  <si>
-    <t>f_ug_cooperatives.xlsx</t>
   </si>
   <si>
     <t>Cooperatives in the Upper Gulf of California</t>
@@ -2285,9 +2276,6 @@
     <t>Avisos de arrib, catch landings cooperatives San Felipe</t>
   </si>
   <si>
-    <t>f_ug_grupo_tecnico_curvina.xlsx</t>
-  </si>
-  <si>
     <t>Technical group of corvina</t>
   </si>
   <si>
@@ -2316,9 +2304,6 @@
     <t>008</t>
   </si>
   <si>
-    <t>f_ug_buyers_aldaz.xlsx</t>
-  </si>
-  <si>
     <t>Buyer's dataset in the Upper Gulf of California (Aldaz)</t>
   </si>
   <si>
@@ -2347,9 +2332,6 @@
     <t>009</t>
   </si>
   <si>
-    <t>f_ug_buyers_ochoa.xlsx</t>
-  </si>
-  <si>
     <t>Buyer's dataset in the Upper Gulf of California (Ochoa)</t>
   </si>
   <si>
@@ -2374,9 +2356,6 @@
     <t>010</t>
   </si>
   <si>
-    <t>f_ug_conapesca_2000_2008.xslx</t>
-  </si>
-  <si>
     <t>Upper Gulf of California fisheries statistics (2000 - 2008)</t>
   </si>
   <si>
@@ -2398,9 +2377,6 @@
     <t>011</t>
   </si>
   <si>
-    <t>f_ug_conapesca.xslx</t>
-  </si>
-  <si>
     <t>Upper Gulf of California fisheries statistics</t>
   </si>
   <si>
@@ -2417,9 +2393,6 @@
   </si>
   <si>
     <t>CONAPESCA catch data | Gulf corvina</t>
-  </si>
-  <si>
-    <t>f_ug_acoustics_corvina_length.xlsx</t>
   </si>
   <si>
     <t>Cota-Nieto, Juan Jose; Jimenez-Esquivel, Victoria; Mascareñas-Osorio, Ismael (2016): Bahia Magdalena: habitat diversity sustains fisheries. In dataMares Project: Fisheries. UC San Diego Library Digital Collections.</t>
@@ -4012,8 +3985,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4139,7 +4112,7 @@
         <v>485</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="D2" s="17" t="s">
         <v>403</v>
@@ -4179,27 +4152,27 @@
         <v>633</v>
       </c>
       <c r="Q2" s="22" t="s">
-        <v>795</v>
+        <v>786</v>
       </c>
       <c r="R2" s="27"/>
       <c r="S2" s="22" t="s">
         <v>629</v>
       </c>
       <c r="T2" s="23" t="s">
+        <v>699</v>
+      </c>
+      <c r="U2" s="22" t="s">
         <v>700</v>
-      </c>
-      <c r="U2" s="22" t="s">
-        <v>701</v>
       </c>
       <c r="V2" s="22" t="s">
         <v>641</v>
       </c>
       <c r="W2" s="17" t="s">
-        <v>830</v>
+        <v>821</v>
       </c>
       <c r="X2" s="17"/>
       <c r="Y2" s="17" t="s">
-        <v>840</v>
+        <v>831</v>
       </c>
       <c r="Z2" s="17"/>
       <c r="AA2" s="19" t="s">
@@ -4217,7 +4190,7 @@
         <v>485</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="D3" s="17" t="s">
         <v>403</v>
@@ -4232,7 +4205,7 @@
         <v>433</v>
       </c>
       <c r="H3" s="17" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="I3" s="17" t="s">
         <v>638</v>
@@ -4250,35 +4223,35 @@
         <v>626</v>
       </c>
       <c r="N3" s="17" t="s">
+        <v>701</v>
+      </c>
+      <c r="O3" s="17" t="s">
         <v>702</v>
       </c>
-      <c r="O3" s="17" t="s">
+      <c r="P3" s="17" t="s">
         <v>703</v>
       </c>
-      <c r="P3" s="17" t="s">
+      <c r="Q3" s="22" t="s">
+        <v>802</v>
+      </c>
+      <c r="S3" s="22" t="s">
+        <v>709</v>
+      </c>
+      <c r="T3" s="23" t="s">
         <v>704</v>
       </c>
-      <c r="Q3" s="22" t="s">
-        <v>811</v>
-      </c>
-      <c r="S3" s="22" t="s">
-        <v>710</v>
-      </c>
-      <c r="T3" s="23" t="s">
+      <c r="U3" s="22" t="s">
         <v>705</v>
-      </c>
-      <c r="U3" s="22" t="s">
-        <v>706</v>
       </c>
       <c r="V3" s="22"/>
       <c r="W3" s="17" t="s">
+        <v>707</v>
+      </c>
+      <c r="X3" s="17" t="s">
         <v>708</v>
       </c>
-      <c r="X3" s="17" t="s">
-        <v>709</v>
-      </c>
       <c r="Y3" s="17" t="s">
-        <v>841</v>
+        <v>832</v>
       </c>
       <c r="Z3" s="17"/>
       <c r="AA3" s="17" t="s">
@@ -4295,15 +4268,9 @@
       <c r="B4" s="17" t="s">
         <v>485</v>
       </c>
-      <c r="C4" s="17" t="s">
-        <v>726</v>
-      </c>
-      <c r="D4" s="17" t="s">
-        <v>403</v>
-      </c>
-      <c r="E4" s="17" t="s">
-        <v>473</v>
-      </c>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
       <c r="F4" s="17" t="s">
         <v>358</v>
       </c>
@@ -4311,54 +4278,54 @@
         <v>433</v>
       </c>
       <c r="H4" s="17" t="s">
+        <v>725</v>
+      </c>
+      <c r="I4" s="17" t="s">
+        <v>726</v>
+      </c>
+      <c r="J4" s="17" t="s">
+        <v>726</v>
+      </c>
+      <c r="K4" s="17" t="s">
         <v>727</v>
-      </c>
-      <c r="I4" s="17" t="s">
-        <v>728</v>
-      </c>
-      <c r="J4" s="17" t="s">
-        <v>728</v>
-      </c>
-      <c r="K4" s="17" t="s">
-        <v>729</v>
       </c>
       <c r="L4" s="17" t="s">
         <v>623</v>
       </c>
       <c r="M4" s="17"/>
       <c r="N4" s="17" t="s">
-        <v>802</v>
+        <v>793</v>
       </c>
       <c r="O4" s="17" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="P4" s="17" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="Q4" s="22"/>
       <c r="R4" s="27" t="s">
-        <v>812</v>
+        <v>803</v>
       </c>
       <c r="S4" s="22" t="s">
-        <v>828</v>
+        <v>819</v>
       </c>
       <c r="T4" s="23" t="s">
+        <v>730</v>
+      </c>
+      <c r="U4" s="22" t="s">
+        <v>731</v>
+      </c>
+      <c r="V4" s="22" t="s">
         <v>732</v>
-      </c>
-      <c r="U4" s="22" t="s">
-        <v>733</v>
-      </c>
-      <c r="V4" s="22" t="s">
-        <v>734</v>
       </c>
       <c r="W4" s="17"/>
       <c r="X4" s="18"/>
       <c r="Y4" s="17" t="s">
-        <v>842</v>
+        <v>833</v>
       </c>
       <c r="Z4" s="17"/>
       <c r="AA4" s="19" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
       <c r="AB4" s="19"/>
       <c r="AC4" s="18"/>
@@ -4371,7 +4338,7 @@
         <v>485</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="D5" s="17" t="s">
         <v>403</v>
@@ -4386,7 +4353,7 @@
         <v>433</v>
       </c>
       <c r="H5" s="17" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="I5" s="17" t="s">
         <v>630</v>
@@ -4411,16 +4378,16 @@
         <v>646</v>
       </c>
       <c r="Q5" s="22" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="S5" s="22" t="s">
         <v>642</v>
       </c>
       <c r="T5" s="22" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="U5" s="22" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="V5" s="22" t="s">
         <v>647</v>
@@ -4430,10 +4397,10 @@
       </c>
       <c r="X5" s="17"/>
       <c r="Y5" s="17" t="s">
-        <v>843</v>
+        <v>834</v>
       </c>
       <c r="Z5" s="17" t="s">
-        <v>810</v>
+        <v>801</v>
       </c>
       <c r="AA5" s="17"/>
       <c r="AB5" s="17"/>
@@ -4446,7 +4413,7 @@
         <v>485</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="D6" s="17" t="s">
         <v>403</v>
@@ -4488,27 +4455,27 @@
         <v>654</v>
       </c>
       <c r="Q6" s="22" t="s">
-        <v>813</v>
+        <v>804</v>
       </c>
       <c r="R6" s="27"/>
       <c r="S6" s="22" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="T6" s="22" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="U6" s="22" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="V6" s="25" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="W6" s="17" t="s">
         <v>649</v>
       </c>
       <c r="X6" s="17"/>
       <c r="Y6" s="17" t="s">
-        <v>844</v>
+        <v>835</v>
       </c>
       <c r="Z6" s="17"/>
       <c r="AA6" s="17"/>
@@ -4563,27 +4530,27 @@
         <v>624</v>
       </c>
       <c r="Q7" s="24" t="s">
-        <v>814</v>
+        <v>805</v>
       </c>
       <c r="R7" s="27"/>
       <c r="S7" s="24" t="s">
         <v>657</v>
       </c>
       <c r="T7" s="22" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="U7" s="22" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="V7" s="24"/>
       <c r="W7" s="3" t="s">
         <v>658</v>
       </c>
       <c r="X7" s="3" t="s">
-        <v>839</v>
+        <v>830</v>
       </c>
       <c r="Y7" s="3" t="s">
-        <v>845</v>
+        <v>836</v>
       </c>
       <c r="Z7" s="3"/>
       <c r="AA7" s="3"/>
@@ -4622,7 +4589,7 @@
         <v>667</v>
       </c>
       <c r="K8" s="3" t="s">
-        <v>809</v>
+        <v>800</v>
       </c>
       <c r="L8" s="17" t="s">
         <v>623</v>
@@ -4631,7 +4598,7 @@
         <v>626</v>
       </c>
       <c r="N8" s="3" t="s">
-        <v>803</v>
+        <v>794</v>
       </c>
       <c r="O8" s="3" t="s">
         <v>668</v>
@@ -4640,53 +4607,44 @@
         <v>669</v>
       </c>
       <c r="Q8" s="24" t="s">
-        <v>815</v>
+        <v>806</v>
       </c>
       <c r="R8" s="27"/>
       <c r="S8" s="24" t="s">
         <v>665</v>
       </c>
       <c r="T8" s="24" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="U8" s="22" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="V8" s="24" t="s">
         <v>670</v>
       </c>
       <c r="W8" s="3" t="s">
-        <v>831</v>
+        <v>822</v>
       </c>
       <c r="X8" s="3"/>
       <c r="Y8" s="3" t="s">
-        <v>846</v>
+        <v>837</v>
       </c>
       <c r="Z8" s="3"/>
       <c r="AA8" s="3" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="AB8" s="3" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="AC8"/>
     </row>
     <row r="9" spans="1:29" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="17" t="s">
-        <v>759</v>
+        <v>755</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>485</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>794</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>403</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>473</v>
-      </c>
       <c r="F9" s="3" t="s">
         <v>358</v>
       </c>
@@ -4694,7 +4652,7 @@
         <v>433</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
       <c r="I9" s="17" t="s">
         <v>638</v>
@@ -4703,58 +4661,49 @@
         <v>623</v>
       </c>
       <c r="N9" s="3" t="s">
+        <v>735</v>
+      </c>
+      <c r="O9" s="3" t="s">
+        <v>736</v>
+      </c>
+      <c r="P9" s="3" t="s">
         <v>737</v>
       </c>
-      <c r="O9" s="3" t="s">
+      <c r="Q9" s="24" t="s">
+        <v>727</v>
+      </c>
+      <c r="R9" s="27" t="s">
+        <v>807</v>
+      </c>
+      <c r="S9" s="24" t="s">
         <v>738</v>
       </c>
-      <c r="P9" s="3" t="s">
+      <c r="T9" s="24" t="s">
         <v>739</v>
       </c>
-      <c r="Q9" s="24" t="s">
-        <v>729</v>
-      </c>
-      <c r="R9" s="27" t="s">
-        <v>816</v>
-      </c>
-      <c r="S9" s="24" t="s">
+      <c r="U9" s="24" t="s">
+        <v>789</v>
+      </c>
+      <c r="V9" s="24" t="s">
         <v>740</v>
       </c>
-      <c r="T9" s="24" t="s">
-        <v>741</v>
-      </c>
-      <c r="U9" s="24" t="s">
-        <v>798</v>
-      </c>
-      <c r="V9" s="24" t="s">
-        <v>742</v>
-      </c>
       <c r="W9" s="3" t="s">
-        <v>832</v>
+        <v>823</v>
       </c>
       <c r="X9" s="17" t="s">
-        <v>800</v>
+        <v>791</v>
       </c>
       <c r="Y9" s="3" t="s">
-        <v>847</v>
+        <v>838</v>
       </c>
     </row>
     <row r="10" spans="1:29" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="17" t="s">
-        <v>769</v>
+        <v>764</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>485</v>
       </c>
-      <c r="C10" s="3" t="s">
-        <v>676</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>403</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>473</v>
-      </c>
       <c r="F10" s="3" t="s">
         <v>358</v>
       </c>
@@ -4765,7 +4714,7 @@
         <v>672</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>817</v>
+        <v>808</v>
       </c>
       <c r="J10" s="17" t="s">
         <v>635</v>
@@ -4786,44 +4735,35 @@
         <v>675</v>
       </c>
       <c r="R10" s="27" t="s">
-        <v>821</v>
+        <v>812</v>
       </c>
       <c r="S10" s="24" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="T10" s="24" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="U10" s="22" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="V10" s="24" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="W10" s="3" t="s">
-        <v>833</v>
+        <v>824</v>
       </c>
       <c r="Y10" s="3" t="s">
-        <v>848</v>
+        <v>839</v>
       </c>
       <c r="AC10" s="18"/>
     </row>
     <row r="11" spans="1:29" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="17" t="s">
-        <v>778</v>
+        <v>772</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>485</v>
       </c>
-      <c r="C11" s="3" t="s">
-        <v>760</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>403</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>473</v>
-      </c>
       <c r="F11" s="3" t="s">
         <v>358</v>
       </c>
@@ -4831,10 +4771,10 @@
         <v>433</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>761</v>
+        <v>756</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>817</v>
+        <v>808</v>
       </c>
       <c r="J11" s="17" t="s">
         <v>635</v>
@@ -4847,53 +4787,44 @@
       </c>
       <c r="M11" s="17"/>
       <c r="N11" s="3" t="s">
+        <v>757</v>
+      </c>
+      <c r="O11" s="3" t="s">
+        <v>758</v>
+      </c>
+      <c r="P11" s="3" t="s">
+        <v>759</v>
+      </c>
+      <c r="R11" s="27" t="s">
+        <v>813</v>
+      </c>
+      <c r="S11" s="24" t="s">
+        <v>760</v>
+      </c>
+      <c r="T11" s="24" t="s">
+        <v>761</v>
+      </c>
+      <c r="U11" s="22" t="s">
         <v>762</v>
       </c>
-      <c r="O11" s="3" t="s">
+      <c r="V11" s="24" t="s">
         <v>763</v>
       </c>
-      <c r="P11" s="3" t="s">
-        <v>764</v>
-      </c>
-      <c r="R11" s="27" t="s">
-        <v>822</v>
-      </c>
-      <c r="S11" s="24" t="s">
-        <v>765</v>
-      </c>
-      <c r="T11" s="24" t="s">
-        <v>766</v>
-      </c>
-      <c r="U11" s="22" t="s">
-        <v>767</v>
-      </c>
-      <c r="V11" s="24" t="s">
-        <v>768</v>
-      </c>
       <c r="W11" s="3" t="s">
-        <v>834</v>
+        <v>825</v>
       </c>
       <c r="Y11" s="3" t="s">
-        <v>849</v>
+        <v>840</v>
       </c>
       <c r="AC11" s="3"/>
     </row>
     <row r="12" spans="1:29" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="17" t="s">
-        <v>786</v>
+        <v>779</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>485</v>
       </c>
-      <c r="C12" s="3" t="s">
-        <v>770</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>403</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>473</v>
-      </c>
       <c r="F12" s="3" t="s">
         <v>358</v>
       </c>
@@ -4901,13 +4832,13 @@
         <v>433</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>771</v>
+        <v>765</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>817</v>
+        <v>808</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>817</v>
+        <v>808</v>
       </c>
       <c r="K12" s="17" t="s">
         <v>651</v>
@@ -4917,58 +4848,49 @@
       </c>
       <c r="M12" s="17"/>
       <c r="N12" s="3" t="s">
-        <v>772</v>
+        <v>766</v>
       </c>
       <c r="O12" s="3" t="s">
-        <v>773</v>
+        <v>767</v>
       </c>
       <c r="P12" s="3" t="s">
-        <v>774</v>
+        <v>768</v>
       </c>
       <c r="R12" s="27" t="s">
-        <v>823</v>
+        <v>814</v>
       </c>
       <c r="S12" s="24" t="s">
-        <v>748</v>
+        <v>745</v>
       </c>
       <c r="T12" s="24" t="s">
-        <v>796</v>
+        <v>787</v>
       </c>
       <c r="U12" s="22" t="s">
-        <v>767</v>
+        <v>762</v>
       </c>
       <c r="V12" s="24" t="s">
-        <v>775</v>
+        <v>769</v>
       </c>
       <c r="W12" s="3" t="s">
-        <v>785</v>
+        <v>778</v>
       </c>
       <c r="Y12" s="3" t="s">
-        <v>850</v>
+        <v>841</v>
       </c>
       <c r="AA12" s="3" t="s">
-        <v>776</v>
+        <v>770</v>
       </c>
       <c r="AB12" s="3" t="s">
-        <v>777</v>
+        <v>771</v>
       </c>
     </row>
     <row r="13" spans="1:29" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="17" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>485</v>
       </c>
-      <c r="C13" s="3" t="s">
-        <v>779</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>403</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>473</v>
-      </c>
       <c r="F13" s="3" t="s">
         <v>358</v>
       </c>
@@ -4976,13 +4898,13 @@
         <v>433</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>780</v>
+        <v>773</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>817</v>
+        <v>808</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>817</v>
+        <v>808</v>
       </c>
       <c r="K13" s="3" t="s">
         <v>651</v>
@@ -4991,52 +4913,43 @@
         <v>623</v>
       </c>
       <c r="N13" s="20" t="s">
-        <v>781</v>
+        <v>774</v>
       </c>
       <c r="O13" s="3" t="s">
-        <v>782</v>
+        <v>775</v>
       </c>
       <c r="P13" s="3" t="s">
-        <v>783</v>
+        <v>776</v>
       </c>
       <c r="R13" s="27" t="s">
-        <v>819</v>
+        <v>810</v>
       </c>
       <c r="S13" s="24" t="s">
-        <v>748</v>
+        <v>745</v>
       </c>
       <c r="T13" s="24" t="s">
-        <v>796</v>
+        <v>787</v>
       </c>
       <c r="U13" s="22" t="s">
-        <v>767</v>
+        <v>762</v>
       </c>
       <c r="V13" s="24" t="s">
-        <v>784</v>
+        <v>777</v>
       </c>
       <c r="W13" s="3" t="s">
-        <v>785</v>
+        <v>778</v>
       </c>
       <c r="Y13" s="3" t="s">
-        <v>850</v>
+        <v>841</v>
       </c>
     </row>
     <row r="14" spans="1:29" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="17" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>485</v>
       </c>
-      <c r="C14" s="3" t="s">
-        <v>787</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>403</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>473</v>
-      </c>
       <c r="F14" s="3" t="s">
         <v>358</v>
       </c>
@@ -5044,10 +4957,10 @@
         <v>433</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>788</v>
+        <v>780</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>817</v>
+        <v>808</v>
       </c>
       <c r="J14" s="17" t="s">
         <v>635</v>
@@ -5056,52 +4969,43 @@
         <v>623</v>
       </c>
       <c r="N14" s="3" t="s">
-        <v>789</v>
+        <v>781</v>
       </c>
       <c r="O14" s="3" t="s">
-        <v>790</v>
+        <v>782</v>
       </c>
       <c r="P14" s="3" t="s">
-        <v>791</v>
+        <v>783</v>
       </c>
       <c r="R14" s="27" t="s">
-        <v>824</v>
+        <v>815</v>
       </c>
       <c r="S14" s="24" t="s">
-        <v>748</v>
+        <v>745</v>
       </c>
       <c r="T14" s="24" t="s">
-        <v>766</v>
+        <v>761</v>
       </c>
       <c r="U14" s="22" t="s">
-        <v>767</v>
+        <v>762</v>
       </c>
       <c r="V14" s="24" t="s">
-        <v>792</v>
+        <v>784</v>
       </c>
       <c r="W14" s="3" t="s">
-        <v>793</v>
+        <v>785</v>
       </c>
       <c r="Y14" s="3" t="s">
-        <v>851</v>
+        <v>842</v>
       </c>
     </row>
     <row r="15" spans="1:29" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="17" t="s">
-        <v>804</v>
+        <v>795</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>485</v>
       </c>
-      <c r="C15" s="3" t="s">
-        <v>743</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>403</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>473</v>
-      </c>
       <c r="F15" s="3" t="s">
         <v>358</v>
       </c>
@@ -5109,64 +5013,58 @@
         <v>433</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>744</v>
+        <v>741</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>817</v>
+        <v>808</v>
       </c>
       <c r="J15" s="3" t="s">
-        <v>817</v>
+        <v>808</v>
       </c>
       <c r="K15" s="3" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
       <c r="L15" s="17" t="s">
         <v>623</v>
       </c>
       <c r="N15" s="3" t="s">
+        <v>742</v>
+      </c>
+      <c r="O15" s="3" t="s">
+        <v>743</v>
+      </c>
+      <c r="P15" s="3" t="s">
+        <v>744</v>
+      </c>
+      <c r="R15" s="27" t="s">
+        <v>816</v>
+      </c>
+      <c r="S15" s="24" t="s">
         <v>745</v>
       </c>
-      <c r="O15" s="3" t="s">
+      <c r="T15" s="24" t="s">
+        <v>787</v>
+      </c>
+      <c r="V15" s="24" t="s">
         <v>746</v>
       </c>
-      <c r="P15" s="3" t="s">
-        <v>747</v>
-      </c>
-      <c r="R15" s="27" t="s">
-        <v>825</v>
-      </c>
-      <c r="S15" s="24" t="s">
-        <v>748</v>
-      </c>
-      <c r="T15" s="24" t="s">
-        <v>796</v>
-      </c>
-      <c r="V15" s="24" t="s">
-        <v>749</v>
-      </c>
       <c r="W15" s="3" t="s">
-        <v>835</v>
+        <v>826</v>
       </c>
       <c r="Y15" s="3" t="s">
-        <v>852</v>
+        <v>843</v>
       </c>
     </row>
     <row r="16" spans="1:29" s="18" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="17" t="s">
-        <v>805</v>
+        <v>796</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>485</v>
       </c>
-      <c r="C16" s="3" t="s">
-        <v>750</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>403</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>473</v>
-      </c>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
       <c r="F16" s="3" t="s">
         <v>358</v>
       </c>
@@ -5174,13 +5072,13 @@
         <v>433</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>751</v>
+        <v>747</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>818</v>
+        <v>809</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>817</v>
+        <v>808</v>
       </c>
       <c r="K16" s="3"/>
       <c r="L16" s="17" t="s">
@@ -5188,55 +5086,55 @@
       </c>
       <c r="M16" s="3"/>
       <c r="N16" s="3" t="s">
-        <v>752</v>
+        <v>748</v>
       </c>
       <c r="O16" s="3" t="s">
-        <v>753</v>
+        <v>749</v>
       </c>
       <c r="P16" s="3" t="s">
-        <v>754</v>
+        <v>750</v>
       </c>
       <c r="Q16" s="24"/>
       <c r="R16" s="27" t="s">
-        <v>820</v>
+        <v>811</v>
       </c>
       <c r="S16" s="24" t="s">
-        <v>755</v>
+        <v>751</v>
       </c>
       <c r="T16" s="24" t="s">
-        <v>797</v>
+        <v>788</v>
       </c>
       <c r="U16" s="24" t="s">
-        <v>799</v>
+        <v>790</v>
       </c>
       <c r="V16" s="24" t="s">
-        <v>756</v>
+        <v>752</v>
       </c>
       <c r="W16" s="3" t="s">
-        <v>836</v>
+        <v>827</v>
       </c>
       <c r="X16" s="3"/>
       <c r="Y16" s="3" t="s">
-        <v>853</v>
+        <v>844</v>
       </c>
       <c r="Z16" s="3"/>
       <c r="AA16" s="3" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
       <c r="AB16" s="3" t="s">
-        <v>758</v>
+        <v>754</v>
       </c>
       <c r="AC16" s="3"/>
     </row>
     <row r="17" spans="1:28" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="17" t="s">
-        <v>806</v>
+        <v>797</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>485</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>403</v>
@@ -5251,10 +5149,10 @@
         <v>433</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>827</v>
+        <v>818</v>
       </c>
       <c r="J17" s="17" t="s">
         <v>627</v>
@@ -5269,48 +5167,48 @@
         <v>626</v>
       </c>
       <c r="N17" s="3" t="s">
+        <v>681</v>
+      </c>
+      <c r="O17" s="3" t="s">
         <v>682</v>
       </c>
-      <c r="O17" s="3" t="s">
+      <c r="P17" s="3" t="s">
         <v>683</v>
       </c>
-      <c r="P17" s="3" t="s">
-        <v>684</v>
-      </c>
       <c r="Q17" s="24" t="s">
-        <v>826</v>
+        <v>817</v>
       </c>
       <c r="S17" s="24" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="T17" s="24" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="U17" s="22" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="V17" s="24" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="W17" s="3" t="s">
-        <v>837</v>
+        <v>828</v>
       </c>
       <c r="X17" s="3" t="s">
-        <v>801</v>
+        <v>792</v>
       </c>
       <c r="Y17" s="3" t="s">
-        <v>847</v>
+        <v>838</v>
       </c>
     </row>
     <row r="18" spans="1:28" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="17" t="s">
-        <v>807</v>
+        <v>798</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>485</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>403</v>
@@ -5325,7 +5223,7 @@
         <v>433</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="I18" s="17" t="s">
         <v>627</v>
@@ -5340,40 +5238,40 @@
         <v>626</v>
       </c>
       <c r="N18" s="3" t="s">
+        <v>688</v>
+      </c>
+      <c r="O18" s="3" t="s">
         <v>689</v>
       </c>
-      <c r="O18" s="3" t="s">
+      <c r="P18" s="3" t="s">
         <v>690</v>
       </c>
-      <c r="P18" s="3" t="s">
-        <v>691</v>
-      </c>
       <c r="Q18" s="24" t="s">
-        <v>808</v>
+        <v>799</v>
       </c>
       <c r="S18" s="24" t="s">
+        <v>720</v>
+      </c>
+      <c r="T18" s="24" t="s">
         <v>721</v>
       </c>
-      <c r="T18" s="24" t="s">
+      <c r="U18" s="22" t="s">
         <v>722</v>
       </c>
-      <c r="U18" s="22" t="s">
-        <v>723</v>
-      </c>
       <c r="V18" s="24" t="s">
+        <v>692</v>
+      </c>
+      <c r="W18" s="3" t="s">
+        <v>829</v>
+      </c>
+      <c r="Z18" s="3" t="s">
+        <v>820</v>
+      </c>
+      <c r="AA18" s="3" t="s">
         <v>693</v>
       </c>
-      <c r="W18" s="3" t="s">
-        <v>838</v>
-      </c>
-      <c r="Z18" s="3" t="s">
-        <v>829</v>
-      </c>
-      <c r="AA18" s="3" t="s">
+      <c r="AB18" s="3" t="s">
         <v>694</v>
-      </c>
-      <c r="AB18" s="3" t="s">
-        <v>695</v>
       </c>
     </row>
   </sheetData>

</xml_diff>